<commit_message>
updated outputs using new combined table method
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears_11daysout.xlsx
+++ b/output/natl_grandtots_bothyears_11daysout.xlsx
@@ -365,12 +365,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>total_requested_2020</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>total_returned_2016</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_requested_2020</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -404,10 +404,10 @@
         <v>40424921</v>
       </c>
       <c r="B2">
+        <v>61976781</v>
+      </c>
+      <c r="C2">
         <v>21876963</v>
-      </c>
-      <c r="C2">
-        <v>61976781</v>
       </c>
       <c r="D2">
         <v>41395951</v>

</xml_diff>

<commit_message>
added formatting for sharing
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears_11daysout.xlsx
+++ b/output/natl_grandtots_bothyears_11daysout.xlsx
@@ -1,21 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITREPOS\gh_kessler\earlyvoting_election2020\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676E0FD9-A95C-4F2C-991B-B4798487BE58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3000" yWindow="3070" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>total_requested_2016</t>
+  </si>
+  <si>
+    <t>total_requested_2020</t>
+  </si>
+  <si>
+    <t>total_returned_2016</t>
+  </si>
+  <si>
+    <t>total_returned_2020</t>
+  </si>
+  <si>
+    <t>diff_requested</t>
+  </si>
+  <si>
+    <t>pctchg_requested</t>
+  </si>
+  <si>
+    <t>diff_returned</t>
+  </si>
+  <si>
+    <t>pctchg_returned</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,6 +64,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,20 +95,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +201,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +253,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,75 +446,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>total_requested_2016</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>total_requested_2020</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_returned_2016</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>total_returned_2020</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>diff_requested</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>pctchg_requested</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>diff_returned</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>pctchg_returned</t>
-        </is>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
         <v>40424921</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>61976781</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>21876963</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>41395951</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>21551860</v>
       </c>
       <c r="F2">
         <v>53.31</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>19518988</v>
       </c>
       <c r="H2">

</xml_diff>

<commit_message>
IMPORTANT change to null out votes requested comparisons for states that didn't report 2020 figures
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears_11daysout.xlsx
+++ b/output/natl_grandtots_bothyears_11daysout.xlsx
@@ -1,60 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITREPOS\gh_kessler\earlyvoting_election2020\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676E0FD9-A95C-4F2C-991B-B4798487BE58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3070" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>total_requested_2016</t>
-  </si>
-  <si>
-    <t>total_requested_2020</t>
-  </si>
-  <si>
-    <t>total_returned_2016</t>
-  </si>
-  <si>
-    <t>total_returned_2020</t>
-  </si>
-  <si>
-    <t>diff_requested</t>
-  </si>
-  <si>
-    <t>pctchg_requested</t>
-  </si>
-  <si>
-    <t>diff_returned</t>
-  </si>
-  <si>
-    <t>pctchg_returned</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +25,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,34 +49,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -169,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,72 +350,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x2016</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>x2020</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>diff_returned</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pctchg_returned</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>40424921</v>
-      </c>
-      <c r="B2" s="3">
-        <v>61976781</v>
-      </c>
-      <c r="C2" s="3">
+    <row r="2">
+      <c r="A2">
         <v>21876963</v>
       </c>
-      <c r="D2" s="3">
+      <c r="B2">
         <v>41395951</v>
       </c>
-      <c r="E2" s="3">
-        <v>21551860</v>
-      </c>
-      <c r="F2">
-        <v>53.31</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="C2">
         <v>19518988</v>
       </c>
-      <c r="H2">
+      <c r="D2">
         <v>89.22</v>
       </c>
     </row>

</xml_diff>